<commit_message>
team proposal submission to Marmoset
</commit_message>
<xml_diff>
--- a/teams-and-rosters/CS320-Sp24-Teams.xlsx
+++ b/teams-and-rosters/CS320-Sp24-Teams.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\donha\cs320-spring2024\teams-and-rosters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBFC5B31-CDB1-41B8-81E1-5B2B65CA11ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD06F4C4-63E5-4ED1-9C28-41BD7B21813E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="667" windowWidth="26355" windowHeight="14858" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2573" yWindow="2573" windowWidth="21600" windowHeight="11422" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -68,7 +68,7 @@
 &lt;TBD&gt;</t>
   </si>
   <si>
-    <t>In-Class Mentors: Bryce Warner, ???</t>
+    <t>In-Class Mentors: Bryce Warner, Hunter Grimm</t>
   </si>
 </sst>
 </file>
@@ -600,7 +600,7 @@
   <dimension ref="B2:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="B13" sqref="B13:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
team names and members
</commit_message>
<xml_diff>
--- a/teams-and-rosters/CS320-Sp24-Teams.xlsx
+++ b/teams-and-rosters/CS320-Sp24-Teams.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\donha\cs320-spring2024\teams-and-rosters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD06F4C4-63E5-4ED1-9C28-41BD7B21813E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA4DFD2A-9A55-430C-B09A-CA4379B0F320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2573" yWindow="2573" windowWidth="21600" windowHeight="11422" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="765" yWindow="345" windowWidth="14722" windowHeight="11272" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>In-Class Mentors: Bryce Neptune, Rob Wood</t>
   </si>
@@ -34,41 +34,107 @@
   </si>
   <si>
     <t>Section 102 (M-W-F: 1:00 to 1:50)</t>
-  </si>
-  <si>
-    <t>Team 101-1:
-&lt;TBD&gt;</t>
-  </si>
-  <si>
-    <t>Team 101-3:
-&lt;TBD&gt;</t>
-  </si>
-  <si>
-    <t>Team 101-2:
-&lt;TBD&gt;</t>
   </si>
   <si>
     <t>Team 101-4:
 &lt;TBD&gt;</t>
   </si>
   <si>
-    <t>Team 102-1:
-&lt;TBD&gt;</t>
-  </si>
-  <si>
-    <t>Team 102-2:
-&lt;TBD&gt;</t>
-  </si>
-  <si>
-    <t>Team 102-3:
-&lt;TBD&gt;</t>
-  </si>
-  <si>
     <t>Team 102-4:
 &lt;TBD&gt;</t>
   </si>
   <si>
     <t>In-Class Mentors: Bryce Warner, Hunter Grimm</t>
+  </si>
+  <si>
+    <t>Brandon Woodward</t>
+  </si>
+  <si>
+    <t>Emily Culp</t>
+  </si>
+  <si>
+    <t>Emmet Larson</t>
+  </si>
+  <si>
+    <t>Kevin Lindemann</t>
+  </si>
+  <si>
+    <t>Thomas Wakeland</t>
+  </si>
+  <si>
+    <t>Ethan VonStein</t>
+  </si>
+  <si>
+    <t>Alyssa Nelson</t>
+  </si>
+  <si>
+    <t>Matthew Brown</t>
+  </si>
+  <si>
+    <t>Charles Carroll</t>
+  </si>
+  <si>
+    <t>Jakeb Nielsen</t>
+  </si>
+  <si>
+    <t>Carson Mack</t>
+  </si>
+  <si>
+    <t>Jonathan Waight</t>
+  </si>
+  <si>
+    <t>Korbin Dick</t>
+  </si>
+  <si>
+    <t>Spencer Hayes</t>
+  </si>
+  <si>
+    <t>Andrew Loiseau</t>
+  </si>
+  <si>
+    <t>Gabriel Manero</t>
+  </si>
+  <si>
+    <t>Ryon Washington</t>
+  </si>
+  <si>
+    <t>Deborah Amao</t>
+  </si>
+  <si>
+    <t>Zachary Cox</t>
+  </si>
+  <si>
+    <t>Ryan Huber</t>
+  </si>
+  <si>
+    <t>Joshua Byers</t>
+  </si>
+  <si>
+    <t>Ren De Alva</t>
+  </si>
+  <si>
+    <t>Team 101-1:
+RevMetrix Bowler UI</t>
+  </si>
+  <si>
+    <t>Team 102-2:
+RevMetrix Bowler UI</t>
+  </si>
+  <si>
+    <t>Team 102-3:
+TBAG: Apocrypha</t>
+  </si>
+  <si>
+    <t>Team 102-1:
+TBAG: Tea-Bag</t>
+  </si>
+  <si>
+    <t>Team 101-2:
+Productivity Planner</t>
+  </si>
+  <si>
+    <t>Team 101-3:
+TBAG: York County Ghosts</t>
   </si>
 </sst>
 </file>
@@ -599,8 +665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:E13"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -648,40 +714,62 @@
     </row>
     <row r="6" spans="2:6" s="2" customFormat="1" ht="32.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B6" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="12" t="s">
+    </row>
+    <row r="7" spans="2:6" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B7" s="8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
+      <c r="C7" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="E7" s="8"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
+      <c r="B8" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>28</v>
+      </c>
       <c r="E8" s="9"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
+      <c r="B9" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E9" s="10"/>
     </row>
     <row r="10" spans="2:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B10" s="11"/>
+      <c r="B10" s="11" t="s">
+        <v>25</v>
+      </c>
       <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
+      <c r="D10" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="E10" s="11"/>
     </row>
     <row r="11" spans="2:6" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
@@ -696,7 +784,7 @@
     </row>
     <row r="13" spans="2:6" s="4" customFormat="1" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B13" s="16" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
@@ -705,40 +793,62 @@
     </row>
     <row r="14" spans="2:6" ht="32.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B14" s="12" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="2:6" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
+      <c r="B15" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>17</v>
+      </c>
       <c r="E15" s="8"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="8"/>
+      <c r="B16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="E16" s="9"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="9"/>
+      <c r="B17" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>19</v>
+      </c>
       <c r="E17" s="10"/>
     </row>
     <row r="18" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B18" s="14"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
+      <c r="C18" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>20</v>
+      </c>
       <c r="E18" s="14"/>
     </row>
     <row r="19" spans="2:5" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
refactored section 2 teams
</commit_message>
<xml_diff>
--- a/teams-and-rosters/CS320-Sp24-Teams.xlsx
+++ b/teams-and-rosters/CS320-Sp24-Teams.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\donha\cs320-spring2024\teams-and-rosters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F24797A3-76F0-49E4-A9F3-983C70E2C9C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{938173FF-1DFE-49EB-80D4-87EF6B7DDB9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="428" yWindow="8" windowWidth="18667" windowHeight="14775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="368" yWindow="368" windowWidth="26264" windowHeight="15127" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>In-Class Mentors: Bryce Neptune, Rob Wood</t>
   </si>
@@ -36,17 +36,6 @@
     <t>Section 102 (M-W-F: 1:00 to 1:50)</t>
   </si>
   <si>
-    <t>Team 101-4:
-&lt;TBD&gt;</t>
-  </si>
-  <si>
-    <t>Team 102-4:
-&lt;TBD&gt;</t>
-  </si>
-  <si>
-    <t>In-Class Mentors: Bryce Warner, Hunter Grimm</t>
-  </si>
-  <si>
     <t>Brandon Woodward</t>
   </si>
   <si>
@@ -63,12 +52,6 @@
   </si>
   <si>
     <t>Ethan VonStein</t>
-  </si>
-  <si>
-    <t>Alyssa Nelson</t>
-  </si>
-  <si>
-    <t>Matthew Brown</t>
   </si>
   <si>
     <t>Charles Carroll</t>
@@ -125,16 +108,30 @@
 TBAG: Apocrypha</t>
   </si>
   <si>
-    <t>Team 102-1:
-TBAG: Tea-Bag</t>
-  </si>
-  <si>
     <t>Team 101-2:
 Productivity Planner</t>
   </si>
   <si>
     <t>Team 101-3:
 TBAG: York County Ghosts</t>
+  </si>
+  <si>
+    <t>Matt Brown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Team 102-1:
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Team 101-4:
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Team 102-4:
+</t>
+  </si>
+  <si>
+    <t>In-Class Mentors: Bryce Warner, Hunter "Ash" Grimm</t>
   </si>
 </sst>
 </file>
@@ -325,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -362,7 +359,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -374,7 +371,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -681,10 +681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F19"/>
+  <dimension ref="B2:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -732,61 +732,61 @@
     </row>
     <row r="6" spans="2:6" s="2" customFormat="1" ht="32.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B6" s="12" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="B7" s="8" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="18"/>
+        <v>19</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="14"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B8" s="9" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E8" s="9"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B9" s="10" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E9" s="9"/>
     </row>
     <row r="10" spans="2:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B10" s="11" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="11" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E10" s="11"/>
     </row>
@@ -802,7 +802,7 @@
     </row>
     <row r="13" spans="2:6" s="4" customFormat="1" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B13" s="16" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
@@ -811,65 +811,69 @@
     </row>
     <row r="14" spans="2:6" ht="32.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B14" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="15" spans="2:6" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B15" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="8" t="s">
+      <c r="B15" s="14"/>
+      <c r="C15" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="14"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B16" s="9"/>
+      <c r="C16" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="9"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B17" s="9"/>
+      <c r="C17" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="9"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B18" s="18"/>
+      <c r="C18" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="18"/>
+    </row>
+    <row r="19" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B19" s="19"/>
+      <c r="C19" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" s="8"/>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B16" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="9"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B17" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="10"/>
-    </row>
-    <row r="18" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B18" s="14"/>
-      <c r="C18" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18" s="14"/>
-    </row>
-    <row r="19" spans="2:5" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+      <c r="E19" s="19"/>
+    </row>
+    <row r="20" spans="2:5" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="B2:E2"/>

</xml_diff>